<commit_message>
tambah database di mst global dan update mst employee with pciture
</commit_message>
<xml_diff>
--- a/documentation/RDBMS DESIGN.xlsx
+++ b/documentation/RDBMS DESIGN.xlsx
@@ -1,20 +1,20 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23801"/>
-  <workbookPr/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+  <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Side Project\Emma Website\emma-project\documentation\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Emma\emma-project\documentation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EC819706-BFD0-4677-AB57-EFED8B55669F}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-105" yWindow="-105" windowWidth="23250" windowHeight="12570" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Master" sheetId="1" r:id="rId1"/>
     <sheet name="All Table List" sheetId="3" r:id="rId2"/>
+    <sheet name="Postgree Query" sheetId="4" r:id="rId3"/>
   </sheets>
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Master!$B$10:$I$44</definedName>
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="372" uniqueCount="106">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="441" uniqueCount="116">
   <si>
     <t>EMMA RDBMS DESIGN</t>
   </si>
@@ -136,12 +136,6 @@
     <t>first_name</t>
   </si>
   <si>
-    <t>second_name</t>
-  </si>
-  <si>
-    <t>third_name</t>
-  </si>
-  <si>
     <t>id_card</t>
   </si>
   <si>
@@ -347,12 +341,48 @@
   </si>
   <si>
     <t>Deskripsi Global Code</t>
+  </si>
+  <si>
+    <t>middle_name</t>
+  </si>
+  <si>
+    <t>last_name</t>
+  </si>
+  <si>
+    <t>ALTER TABLE public.mst_global ADD COLUMN</t>
+  </si>
+  <si>
+    <t>character varying(15)</t>
+  </si>
+  <si>
+    <t>character varying(300)</t>
+  </si>
+  <si>
+    <t>character varying(100)</t>
+  </si>
+  <si>
+    <t>character varying(20)</t>
+  </si>
+  <si>
+    <t>interger</t>
+  </si>
+  <si>
+    <t>timestamp without zone</t>
+  </si>
+  <si>
+    <t>character varying(30)</t>
+  </si>
+  <si>
+    <t>;</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> </t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -611,25 +641,10 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -637,65 +652,80 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="5" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="4" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="5" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -737,14 +767,14 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{48491D98-FE11-4211-B6B2-FB10EC85A54B}" name="Table1" displayName="Table1" ref="C3:G15" totalsRowShown="0" headerRowDxfId="2" dataDxfId="1">
-  <autoFilter ref="C3:G15" xr:uid="{5BCB4884-F06C-4E62-B7F8-191EA6E8E26E}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table1" displayName="Table1" ref="C3:G15" totalsRowShown="0" headerRowDxfId="6" dataDxfId="5">
+  <autoFilter ref="C3:G15"/>
   <tableColumns count="5">
-    <tableColumn id="1" xr3:uid="{434A7D21-F4C6-4F31-B0A1-22D22F72E321}" name="Table Type" dataDxfId="6"/>
-    <tableColumn id="2" xr3:uid="{A1CBE243-A5C5-4647-8B0B-3CE257A7F038}" name="Table Code" dataDxfId="5"/>
-    <tableColumn id="3" xr3:uid="{8341F95D-12E8-44B0-9214-802DCCA5ED43}" name="Table Name" dataDxfId="4"/>
-    <tableColumn id="4" xr3:uid="{373CDFCD-3E23-49BB-AB72-C99914736A25}" name="isUsed?" dataDxfId="3"/>
-    <tableColumn id="8" xr3:uid="{F99BF06A-E938-418A-8157-C7B00078657E}" name="Note" dataDxfId="0"/>
+    <tableColumn id="1" name="Table Type" dataDxfId="4"/>
+    <tableColumn id="2" name="Table Code" dataDxfId="3"/>
+    <tableColumn id="3" name="Table Name" dataDxfId="2"/>
+    <tableColumn id="4" name="isUsed?" dataDxfId="1"/>
+    <tableColumn id="8" name="Note" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -1012,278 +1042,279 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:T44"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView topLeftCell="J4" workbookViewId="0">
+      <selection activeCell="M11" sqref="M11:N24"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="4" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="4" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="7.88671875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="7.85546875" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="14" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="11.21875" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="14.109375" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="13.77734375" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="12.21875" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="17.21875" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="66.109375" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="3.44140625" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="11.33203125" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="11.21875" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="9.6640625" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="9.33203125" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="7.77734375" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="12.77734375" bestFit="1" customWidth="1"/>
-    <col min="19" max="19" width="34.6640625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="11.28515625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="14.140625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="13.7109375" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="12.28515625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="17.28515625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="66.140625" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="3.42578125" bestFit="1" customWidth="1"/>
+    <col min="13" max="14" width="11.28515625" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="9.7109375" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="9.28515625" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="7.7109375" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="12.7109375" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="34.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:20" x14ac:dyDescent="0.3">
-      <c r="A1" s="12"/>
-    </row>
-    <row r="2" spans="1:20" ht="17.399999999999999" x14ac:dyDescent="0.3">
-      <c r="B2" s="21" t="s">
+    <row r="1" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A1" s="7"/>
+    </row>
+    <row r="2" spans="1:20" ht="18" x14ac:dyDescent="0.25">
+      <c r="B2" s="27" t="s">
         <v>0</v>
       </c>
-      <c r="C2" s="22"/>
-      <c r="D2" s="22"/>
-      <c r="E2" s="22"/>
-      <c r="F2" s="22"/>
-      <c r="G2" s="22"/>
-      <c r="H2" s="22"/>
-      <c r="I2" s="23"/>
+      <c r="C2" s="28"/>
+      <c r="D2" s="28"/>
+      <c r="E2" s="28"/>
+      <c r="F2" s="28"/>
+      <c r="G2" s="28"/>
+      <c r="H2" s="28"/>
+      <c r="I2" s="29"/>
       <c r="J2" s="2"/>
     </row>
-    <row r="3" spans="1:20" ht="17.399999999999999" x14ac:dyDescent="0.3">
-      <c r="B3" s="24"/>
-      <c r="C3" s="16"/>
-      <c r="D3" s="16"/>
-      <c r="E3" s="16"/>
-      <c r="F3" s="16"/>
-      <c r="G3" s="16"/>
-      <c r="H3" s="16"/>
-      <c r="I3" s="25"/>
+    <row r="3" spans="1:20" ht="18" x14ac:dyDescent="0.25">
+      <c r="B3" s="30"/>
+      <c r="C3" s="31"/>
+      <c r="D3" s="31"/>
+      <c r="E3" s="31"/>
+      <c r="F3" s="31"/>
+      <c r="G3" s="31"/>
+      <c r="H3" s="31"/>
+      <c r="I3" s="32"/>
       <c r="J3" s="2"/>
     </row>
-    <row r="4" spans="1:20" ht="17.399999999999999" x14ac:dyDescent="0.3">
-      <c r="B4" s="29" t="s">
+    <row r="4" spans="1:20" ht="18" x14ac:dyDescent="0.25">
+      <c r="B4" s="17" t="s">
         <v>1</v>
       </c>
-      <c r="C4" s="30"/>
-      <c r="D4" s="30"/>
-      <c r="E4" s="30"/>
-      <c r="F4" s="30"/>
-      <c r="G4" s="30"/>
-      <c r="H4" s="30"/>
-      <c r="I4" s="31"/>
+      <c r="C4" s="18"/>
+      <c r="D4" s="18"/>
+      <c r="E4" s="18"/>
+      <c r="F4" s="18"/>
+      <c r="G4" s="18"/>
+      <c r="H4" s="18"/>
+      <c r="I4" s="19"/>
       <c r="J4" s="2"/>
     </row>
-    <row r="5" spans="1:20" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B5" s="14"/>
-      <c r="C5" s="15"/>
-      <c r="D5" s="15"/>
-      <c r="E5" s="15"/>
-      <c r="F5" s="15"/>
-      <c r="G5" s="15"/>
-      <c r="H5" s="15"/>
-      <c r="I5" s="26"/>
-      <c r="L5" s="6"/>
-      <c r="M5" s="6"/>
-      <c r="N5" s="6"/>
-      <c r="O5" s="6"/>
-      <c r="P5" s="6"/>
-      <c r="Q5" s="6"/>
-      <c r="R5" s="6"/>
-      <c r="S5" s="6"/>
-      <c r="T5" s="6"/>
-    </row>
-    <row r="6" spans="1:20" x14ac:dyDescent="0.3">
-      <c r="B6" s="27"/>
-      <c r="C6" s="20"/>
-      <c r="D6" s="20"/>
-      <c r="E6" s="20"/>
-      <c r="F6" s="20"/>
-      <c r="G6" s="20"/>
-      <c r="H6" s="20"/>
-      <c r="I6" s="28"/>
+    <row r="5" spans="1:20" ht="17.45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B5" s="20"/>
+      <c r="C5" s="21"/>
+      <c r="D5" s="21"/>
+      <c r="E5" s="21"/>
+      <c r="F5" s="21"/>
+      <c r="G5" s="21"/>
+      <c r="H5" s="21"/>
+      <c r="I5" s="22"/>
+      <c r="L5" s="5"/>
+      <c r="M5" s="5"/>
+      <c r="N5" s="5"/>
+      <c r="O5" s="5"/>
+      <c r="P5" s="5"/>
+      <c r="Q5" s="5"/>
+      <c r="R5" s="5"/>
+      <c r="S5" s="5"/>
+      <c r="T5" s="5"/>
+    </row>
+    <row r="6" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="B6" s="23"/>
+      <c r="C6" s="24"/>
+      <c r="D6" s="24"/>
+      <c r="E6" s="24"/>
+      <c r="F6" s="24"/>
+      <c r="G6" s="24"/>
+      <c r="H6" s="24"/>
+      <c r="I6" s="25"/>
       <c r="J6" s="1"/>
-      <c r="L6" s="6"/>
-      <c r="M6" s="6"/>
-      <c r="N6" s="6"/>
-      <c r="O6" s="6"/>
-      <c r="P6" s="6"/>
-      <c r="Q6" s="6"/>
-      <c r="R6" s="6"/>
-      <c r="S6" s="6"/>
-      <c r="T6" s="6"/>
-    </row>
-    <row r="7" spans="1:20" x14ac:dyDescent="0.3">
-      <c r="B7" s="10"/>
-      <c r="C7" s="10"/>
-      <c r="D7" s="10"/>
-      <c r="E7" s="10"/>
-      <c r="F7" s="10"/>
-      <c r="G7" s="10"/>
-      <c r="H7" s="10"/>
-      <c r="I7" s="10"/>
-      <c r="L7" s="4"/>
-      <c r="M7" s="4"/>
-      <c r="N7" s="4"/>
-      <c r="O7" s="4"/>
-      <c r="P7" s="4"/>
-      <c r="Q7" s="4"/>
-      <c r="R7" s="4"/>
-      <c r="S7" s="4"/>
-    </row>
-    <row r="8" spans="1:20" x14ac:dyDescent="0.3">
-      <c r="B8" s="7" t="s">
+      <c r="L6" s="5"/>
+      <c r="M6" s="5"/>
+      <c r="N6" s="5"/>
+      <c r="O6" s="5"/>
+      <c r="P6" s="5"/>
+      <c r="Q6" s="5"/>
+      <c r="R6" s="5"/>
+      <c r="S6" s="5"/>
+      <c r="T6" s="5"/>
+    </row>
+    <row r="7" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="B7" s="26"/>
+      <c r="C7" s="26"/>
+      <c r="D7" s="26"/>
+      <c r="E7" s="26"/>
+      <c r="F7" s="26"/>
+      <c r="G7" s="26"/>
+      <c r="H7" s="26"/>
+      <c r="I7" s="26"/>
+      <c r="L7" s="33"/>
+      <c r="M7" s="33"/>
+      <c r="N7" s="33"/>
+      <c r="O7" s="33"/>
+      <c r="P7" s="33"/>
+      <c r="Q7" s="33"/>
+      <c r="R7" s="33"/>
+      <c r="S7" s="33"/>
+    </row>
+    <row r="8" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="B8" s="14" t="s">
         <v>23</v>
       </c>
-      <c r="C8" s="8"/>
-      <c r="D8" s="8"/>
-      <c r="E8" s="8"/>
-      <c r="F8" s="8"/>
-      <c r="G8" s="8"/>
-      <c r="H8" s="8"/>
-      <c r="I8" s="9"/>
-      <c r="L8" s="7" t="s">
-        <v>82</v>
-      </c>
-      <c r="M8" s="8"/>
-      <c r="N8" s="8"/>
-      <c r="O8" s="8"/>
-      <c r="P8" s="8"/>
-      <c r="Q8" s="8"/>
-      <c r="R8" s="8"/>
-      <c r="S8" s="9"/>
-    </row>
-    <row r="9" spans="1:20" x14ac:dyDescent="0.3">
-      <c r="B9" s="7" t="s">
+      <c r="C8" s="15"/>
+      <c r="D8" s="15"/>
+      <c r="E8" s="15"/>
+      <c r="F8" s="15"/>
+      <c r="G8" s="15"/>
+      <c r="H8" s="15"/>
+      <c r="I8" s="16"/>
+      <c r="L8" s="14" t="s">
+        <v>80</v>
+      </c>
+      <c r="M8" s="15"/>
+      <c r="N8" s="15"/>
+      <c r="O8" s="15"/>
+      <c r="P8" s="15"/>
+      <c r="Q8" s="15"/>
+      <c r="R8" s="15"/>
+      <c r="S8" s="16"/>
+    </row>
+    <row r="9" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="B9" s="14" t="s">
         <v>30</v>
       </c>
-      <c r="C9" s="8"/>
-      <c r="D9" s="8"/>
-      <c r="E9" s="8"/>
-      <c r="F9" s="8"/>
-      <c r="G9" s="8"/>
-      <c r="H9" s="8"/>
-      <c r="I9" s="9"/>
-      <c r="L9" s="7" t="s">
+      <c r="C9" s="15"/>
+      <c r="D9" s="15"/>
+      <c r="E9" s="15"/>
+      <c r="F9" s="15"/>
+      <c r="G9" s="15"/>
+      <c r="H9" s="15"/>
+      <c r="I9" s="16"/>
+      <c r="L9" s="14" t="s">
         <v>30</v>
       </c>
-      <c r="M9" s="8"/>
-      <c r="N9" s="8"/>
-      <c r="O9" s="8"/>
-      <c r="P9" s="8"/>
-      <c r="Q9" s="8"/>
-      <c r="R9" s="8"/>
-      <c r="S9" s="9"/>
-    </row>
-    <row r="10" spans="1:20" x14ac:dyDescent="0.3">
-      <c r="B10" s="5" t="s">
+      <c r="M9" s="15"/>
+      <c r="N9" s="15"/>
+      <c r="O9" s="15"/>
+      <c r="P9" s="15"/>
+      <c r="Q9" s="15"/>
+      <c r="R9" s="15"/>
+      <c r="S9" s="16"/>
+    </row>
+    <row r="10" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="B10" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="C10" s="5" t="s">
+      <c r="C10" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="D10" s="5" t="s">
+      <c r="D10" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="E10" s="5" t="s">
+      <c r="E10" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="F10" s="5" t="s">
+      <c r="F10" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="G10" s="5" t="s">
+      <c r="G10" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="H10" s="5" t="s">
-        <v>40</v>
-      </c>
-      <c r="I10" s="5" t="s">
-        <v>45</v>
-      </c>
-      <c r="L10" s="5" t="s">
+      <c r="H10" s="4" t="s">
+        <v>38</v>
+      </c>
+      <c r="I10" s="4" t="s">
+        <v>43</v>
+      </c>
+      <c r="L10" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="M10" s="5" t="s">
+      <c r="M10" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="N10" s="5" t="s">
+      <c r="N10" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="O10" s="5" t="s">
+      <c r="O10" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="P10" s="5" t="s">
+      <c r="P10" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="Q10" s="5" t="s">
+      <c r="Q10" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="R10" s="5" t="s">
-        <v>40</v>
-      </c>
-      <c r="S10" s="5" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="11" spans="1:20" x14ac:dyDescent="0.3">
-      <c r="B11" s="11">
+      <c r="R10" s="4" t="s">
+        <v>38</v>
+      </c>
+      <c r="S10" s="4" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="11" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="B11" s="6">
         <v>1</v>
       </c>
-      <c r="C11" s="11" t="s">
+      <c r="C11" s="6" t="s">
         <v>33</v>
       </c>
-      <c r="D11" s="11" t="s">
+      <c r="D11" s="6" t="s">
         <v>13</v>
       </c>
-      <c r="E11" s="32" t="s">
+      <c r="E11" s="12" t="s">
         <v>8</v>
       </c>
-      <c r="F11" s="11" t="s">
-        <v>9</v>
-      </c>
-      <c r="G11" s="32" t="s">
+      <c r="F11" s="6" t="s">
+        <v>9</v>
+      </c>
+      <c r="G11" s="12" t="s">
         <v>8</v>
       </c>
-      <c r="H11" s="11" t="s">
-        <v>9</v>
-      </c>
-      <c r="I11" s="11" t="s">
-        <v>46</v>
-      </c>
-      <c r="L11" s="11">
+      <c r="H11" s="6" t="s">
+        <v>9</v>
+      </c>
+      <c r="I11" s="6" t="s">
+        <v>44</v>
+      </c>
+      <c r="L11" s="6">
         <v>1</v>
       </c>
-      <c r="M11" s="11" t="s">
-        <v>83</v>
-      </c>
-      <c r="N11" s="11" t="s">
+      <c r="M11" s="6" t="s">
+        <v>81</v>
+      </c>
+      <c r="N11" s="6" t="s">
         <v>11</v>
       </c>
-      <c r="O11" s="32" t="s">
+      <c r="O11" s="12" t="s">
         <v>8</v>
       </c>
-      <c r="P11" s="11" t="s">
-        <v>9</v>
-      </c>
-      <c r="Q11" s="32" t="s">
+      <c r="P11" s="6" t="s">
+        <v>9</v>
+      </c>
+      <c r="Q11" s="12" t="s">
         <v>8</v>
       </c>
-      <c r="R11" s="11" t="s">
-        <v>9</v>
-      </c>
-      <c r="S11" s="11" t="s">
-        <v>95</v>
-      </c>
-    </row>
-    <row r="12" spans="1:20" x14ac:dyDescent="0.3">
-      <c r="B12" s="11">
+      <c r="R11" s="6" t="s">
+        <v>9</v>
+      </c>
+      <c r="S11" s="6" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="12" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="B12" s="6">
         <v>2</v>
       </c>
       <c r="C12" s="3" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="D12" s="3" t="s">
         <v>13</v>
@@ -1301,13 +1332,13 @@
         <v>9</v>
       </c>
       <c r="I12" s="3" t="s">
-        <v>51</v>
-      </c>
-      <c r="L12" s="11">
+        <v>49</v>
+      </c>
+      <c r="L12" s="6">
         <v>2</v>
       </c>
-      <c r="M12" s="33" t="s">
-        <v>84</v>
+      <c r="M12" s="13" t="s">
+        <v>82</v>
       </c>
       <c r="N12" s="3" t="s">
         <v>13</v>
@@ -1318,18 +1349,18 @@
       <c r="P12" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="Q12" s="33" t="s">
+      <c r="Q12" s="13" t="s">
         <v>8</v>
       </c>
-      <c r="R12" s="33" t="s">
+      <c r="R12" s="13" t="s">
         <v>8</v>
       </c>
       <c r="S12" s="3" t="s">
-        <v>94</v>
-      </c>
-    </row>
-    <row r="13" spans="1:20" x14ac:dyDescent="0.3">
-      <c r="B13" s="11">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="13" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="B13" s="6">
         <v>3</v>
       </c>
       <c r="C13" s="3" t="s">
@@ -1351,13 +1382,13 @@
         <v>9</v>
       </c>
       <c r="I13" s="3" t="s">
-        <v>47</v>
-      </c>
-      <c r="L13" s="11">
+        <v>45</v>
+      </c>
+      <c r="L13" s="6">
         <v>3</v>
       </c>
       <c r="M13" s="3" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="N13" s="3" t="s">
         <v>16</v>
@@ -1375,15 +1406,15 @@
         <v>9</v>
       </c>
       <c r="S13" s="3" t="s">
-        <v>105</v>
-      </c>
-    </row>
-    <row r="14" spans="1:20" x14ac:dyDescent="0.3">
-      <c r="B14" s="11">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="14" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="B14" s="6">
         <v>4</v>
       </c>
       <c r="C14" s="3" t="s">
-        <v>35</v>
+        <v>104</v>
       </c>
       <c r="D14" s="3" t="s">
         <v>12</v>
@@ -1401,13 +1432,13 @@
         <v>9</v>
       </c>
       <c r="I14" s="3" t="s">
-        <v>48</v>
-      </c>
-      <c r="L14" s="11">
+        <v>46</v>
+      </c>
+      <c r="L14" s="6">
         <v>4</v>
       </c>
       <c r="M14" s="3" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="N14" s="3" t="s">
         <v>12</v>
@@ -1425,15 +1456,15 @@
         <v>9</v>
       </c>
       <c r="S14" s="3" t="s">
-        <v>93</v>
-      </c>
-    </row>
-    <row r="15" spans="1:20" x14ac:dyDescent="0.3">
-      <c r="B15" s="11">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="15" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="B15" s="6">
         <v>5</v>
       </c>
       <c r="C15" s="3" t="s">
-        <v>36</v>
+        <v>105</v>
       </c>
       <c r="D15" s="3" t="s">
         <v>12</v>
@@ -1451,13 +1482,13 @@
         <v>9</v>
       </c>
       <c r="I15" s="3" t="s">
-        <v>49</v>
-      </c>
-      <c r="L15" s="11">
+        <v>47</v>
+      </c>
+      <c r="L15" s="6">
         <v>5</v>
       </c>
       <c r="M15" s="3" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="N15" s="3" t="s">
         <v>12</v>
@@ -1475,15 +1506,15 @@
         <v>9</v>
       </c>
       <c r="S15" s="3" t="s">
-        <v>93</v>
-      </c>
-    </row>
-    <row r="16" spans="1:20" x14ac:dyDescent="0.3">
-      <c r="B16" s="11">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="16" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="B16" s="6">
         <v>6</v>
       </c>
       <c r="C16" s="3" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="D16" s="3" t="s">
         <v>12</v>
@@ -1501,13 +1532,13 @@
         <v>9</v>
       </c>
       <c r="I16" s="3" t="s">
-        <v>50</v>
-      </c>
-      <c r="L16" s="11">
+        <v>48</v>
+      </c>
+      <c r="L16" s="6">
         <v>6</v>
       </c>
       <c r="M16" s="3" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
       <c r="N16" s="3" t="s">
         <v>12</v>
@@ -1525,11 +1556,11 @@
         <v>9</v>
       </c>
       <c r="S16" s="3" t="s">
-        <v>93</v>
-      </c>
-    </row>
-    <row r="17" spans="2:19" x14ac:dyDescent="0.3">
-      <c r="B17" s="11">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="17" spans="2:19" x14ac:dyDescent="0.25">
+      <c r="B17" s="6">
         <v>7</v>
       </c>
       <c r="C17" s="3" t="s">
@@ -1551,16 +1582,16 @@
         <v>9</v>
       </c>
       <c r="I17" s="3" t="s">
-        <v>52</v>
-      </c>
-      <c r="L17" s="11">
+        <v>50</v>
+      </c>
+      <c r="L17" s="6">
         <v>7</v>
       </c>
       <c r="M17" s="3" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="N17" s="3" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="O17" s="3" t="s">
         <v>9</v>
@@ -1575,15 +1606,15 @@
         <v>9</v>
       </c>
       <c r="S17" s="3" t="s">
-        <v>92</v>
-      </c>
-    </row>
-    <row r="18" spans="2:19" x14ac:dyDescent="0.3">
-      <c r="B18" s="11">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="18" spans="2:19" x14ac:dyDescent="0.25">
+      <c r="B18" s="6">
         <v>8</v>
       </c>
-      <c r="C18" s="33" t="s">
-        <v>39</v>
+      <c r="C18" s="13" t="s">
+        <v>37</v>
       </c>
       <c r="D18" s="3" t="s">
         <v>13</v>
@@ -1597,39 +1628,39 @@
       <c r="G18" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="H18" s="33" t="s">
+      <c r="H18" s="13" t="s">
         <v>8</v>
       </c>
       <c r="I18" s="3" t="s">
-        <v>53</v>
-      </c>
-      <c r="L18" s="11">
+        <v>51</v>
+      </c>
+      <c r="L18" s="6">
         <v>8</v>
       </c>
       <c r="M18" s="3" t="s">
+        <v>88</v>
+      </c>
+      <c r="N18" s="3" t="s">
+        <v>102</v>
+      </c>
+      <c r="O18" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="P18" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="Q18" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="R18" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="S18" s="3" t="s">
         <v>90</v>
       </c>
-      <c r="N18" s="3" t="s">
-        <v>104</v>
-      </c>
-      <c r="O18" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="P18" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="Q18" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="R18" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="S18" s="3" t="s">
-        <v>92</v>
-      </c>
-    </row>
-    <row r="19" spans="2:19" x14ac:dyDescent="0.3">
-      <c r="B19" s="11">
+    </row>
+    <row r="19" spans="2:19" x14ac:dyDescent="0.25">
+      <c r="B19" s="6">
         <v>9</v>
       </c>
       <c r="C19" s="3" t="s">
@@ -1651,16 +1682,16 @@
         <v>9</v>
       </c>
       <c r="I19" s="3" t="s">
-        <v>54</v>
-      </c>
-      <c r="L19" s="11">
+        <v>52</v>
+      </c>
+      <c r="L19" s="6">
         <v>9</v>
       </c>
       <c r="M19" s="3" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="N19" s="3" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="O19" s="3" t="s">
         <v>9</v>
@@ -1675,15 +1706,15 @@
         <v>9</v>
       </c>
       <c r="S19" s="3" t="s">
-        <v>92</v>
-      </c>
-    </row>
-    <row r="20" spans="2:19" x14ac:dyDescent="0.3">
-      <c r="B20" s="11">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="20" spans="2:19" x14ac:dyDescent="0.25">
+      <c r="B20" s="6">
         <v>10</v>
       </c>
       <c r="C20" s="3" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="D20" s="3" t="s">
         <v>10</v>
@@ -1701,13 +1732,13 @@
         <v>9</v>
       </c>
       <c r="I20" s="3" t="s">
-        <v>55</v>
-      </c>
-      <c r="L20" s="11">
+        <v>53</v>
+      </c>
+      <c r="L20" s="6">
         <v>10</v>
       </c>
       <c r="M20" s="3" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
       <c r="N20" s="3" t="s">
         <v>16</v>
@@ -1725,15 +1756,15 @@
         <v>9</v>
       </c>
       <c r="S20" s="3" t="s">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="21" spans="2:19" x14ac:dyDescent="0.3">
-      <c r="B21" s="11">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="21" spans="2:19" x14ac:dyDescent="0.25">
+      <c r="B21" s="6">
         <v>11</v>
       </c>
       <c r="C21" s="3" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="D21" s="3" t="s">
         <v>10</v>
@@ -1751,9 +1782,9 @@
         <v>9</v>
       </c>
       <c r="I21" s="3" t="s">
-        <v>56</v>
-      </c>
-      <c r="L21" s="11">
+        <v>54</v>
+      </c>
+      <c r="L21" s="6">
         <v>11</v>
       </c>
       <c r="M21" s="3" t="s">
@@ -1775,11 +1806,11 @@
         <v>9</v>
       </c>
       <c r="S21" s="3" t="s">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="22" spans="2:19" x14ac:dyDescent="0.3">
-      <c r="B22" s="11">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="22" spans="2:19" x14ac:dyDescent="0.25">
+      <c r="B22" s="6">
         <v>12</v>
       </c>
       <c r="C22" s="3" t="s">
@@ -1801,13 +1832,13 @@
         <v>9</v>
       </c>
       <c r="I22" s="3" t="s">
-        <v>57</v>
-      </c>
-      <c r="L22" s="11">
+        <v>55</v>
+      </c>
+      <c r="L22" s="6">
         <v>12</v>
       </c>
       <c r="M22" s="3" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="N22" s="3" t="s">
         <v>10</v>
@@ -1825,15 +1856,15 @@
         <v>9</v>
       </c>
       <c r="S22" s="3" t="s">
-        <v>71</v>
-      </c>
-    </row>
-    <row r="23" spans="2:19" x14ac:dyDescent="0.3">
-      <c r="B23" s="11">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="23" spans="2:19" x14ac:dyDescent="0.25">
+      <c r="B23" s="6">
         <v>13</v>
       </c>
-      <c r="C23" s="33" t="s">
-        <v>43</v>
+      <c r="C23" s="13" t="s">
+        <v>41</v>
       </c>
       <c r="D23" s="3" t="s">
         <v>13</v>
@@ -1847,17 +1878,17 @@
       <c r="G23" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="H23" s="33" t="s">
+      <c r="H23" s="13" t="s">
         <v>8</v>
       </c>
       <c r="I23" s="3" t="s">
-        <v>59</v>
-      </c>
-      <c r="L23" s="11">
+        <v>57</v>
+      </c>
+      <c r="L23" s="6">
         <v>13</v>
       </c>
       <c r="M23" s="3" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
       <c r="N23" s="3" t="s">
         <v>17</v>
@@ -1875,15 +1906,15 @@
         <v>9</v>
       </c>
       <c r="S23" s="3" t="s">
-        <v>72</v>
-      </c>
-    </row>
-    <row r="24" spans="2:19" x14ac:dyDescent="0.3">
-      <c r="B24" s="11">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="24" spans="2:19" x14ac:dyDescent="0.25">
+      <c r="B24" s="6">
         <v>14</v>
       </c>
-      <c r="C24" s="33" t="s">
-        <v>44</v>
+      <c r="C24" s="13" t="s">
+        <v>42</v>
       </c>
       <c r="D24" s="3" t="s">
         <v>13</v>
@@ -1897,17 +1928,17 @@
       <c r="G24" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="H24" s="33" t="s">
+      <c r="H24" s="13" t="s">
         <v>8</v>
       </c>
       <c r="I24" s="3" t="s">
-        <v>58</v>
-      </c>
-      <c r="L24" s="11">
+        <v>56</v>
+      </c>
+      <c r="L24" s="6">
         <v>14</v>
       </c>
       <c r="M24" s="3" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
       <c r="N24" s="3" t="s">
         <v>28</v>
@@ -1925,37 +1956,37 @@
         <v>9</v>
       </c>
       <c r="S24" s="3" t="s">
-        <v>73</v>
-      </c>
-    </row>
-    <row r="25" spans="2:19" x14ac:dyDescent="0.3">
-      <c r="B25" s="11">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="25" spans="2:19" x14ac:dyDescent="0.25">
+      <c r="B25" s="6">
         <v>15</v>
       </c>
       <c r="C25" s="3" t="s">
+        <v>58</v>
+      </c>
+      <c r="D25" s="3" t="s">
+        <v>59</v>
+      </c>
+      <c r="E25" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="F25" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="G25" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="H25" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="I25" s="3" t="s">
         <v>60</v>
       </c>
-      <c r="D25" s="3" t="s">
-        <v>61</v>
-      </c>
-      <c r="E25" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="F25" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="G25" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="H25" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="I25" s="3" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="26" spans="2:19" x14ac:dyDescent="0.3">
-      <c r="B26" s="11">
+    </row>
+    <row r="26" spans="2:19" x14ac:dyDescent="0.25">
+      <c r="B26" s="6">
         <v>16</v>
       </c>
       <c r="C26" s="3" t="s">
@@ -1977,11 +2008,11 @@
         <v>9</v>
       </c>
       <c r="I26" s="3" t="s">
-        <v>63</v>
-      </c>
-    </row>
-    <row r="27" spans="2:19" x14ac:dyDescent="0.3">
-      <c r="B27" s="11">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="27" spans="2:19" x14ac:dyDescent="0.25">
+      <c r="B27" s="6">
         <v>17</v>
       </c>
       <c r="C27" s="3" t="s">
@@ -2003,14 +2034,14 @@
         <v>9</v>
       </c>
       <c r="I27" s="3" t="s">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="28" spans="2:19" x14ac:dyDescent="0.3">
-      <c r="B28" s="11">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="28" spans="2:19" x14ac:dyDescent="0.25">
+      <c r="B28" s="6">
         <v>18</v>
       </c>
-      <c r="C28" s="33" t="s">
+      <c r="C28" s="13" t="s">
         <v>22</v>
       </c>
       <c r="D28" s="3" t="s">
@@ -2025,19 +2056,19 @@
       <c r="G28" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="H28" s="33" t="s">
+      <c r="H28" s="13" t="s">
         <v>8</v>
       </c>
       <c r="I28" s="3" t="s">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="29" spans="2:19" x14ac:dyDescent="0.3">
-      <c r="B29" s="11">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="29" spans="2:19" x14ac:dyDescent="0.25">
+      <c r="B29" s="6">
         <v>19</v>
       </c>
-      <c r="C29" s="33" t="s">
-        <v>74</v>
+      <c r="C29" s="13" t="s">
+        <v>72</v>
       </c>
       <c r="D29" s="3" t="s">
         <v>13</v>
@@ -2045,24 +2076,24 @@
       <c r="E29" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="F29" s="33" t="s">
+      <c r="F29" s="13" t="s">
         <v>8</v>
       </c>
       <c r="G29" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="H29" s="33" t="s">
+      <c r="H29" s="13" t="s">
         <v>8</v>
       </c>
       <c r="I29" s="3" t="s">
-        <v>66</v>
-      </c>
-    </row>
-    <row r="30" spans="2:19" x14ac:dyDescent="0.3">
-      <c r="B30" s="11">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="30" spans="2:19" x14ac:dyDescent="0.25">
+      <c r="B30" s="6">
         <v>20</v>
       </c>
-      <c r="C30" s="33" t="s">
+      <c r="C30" s="13" t="s">
         <v>31</v>
       </c>
       <c r="D30" s="3" t="s">
@@ -2071,24 +2102,24 @@
       <c r="E30" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="F30" s="33" t="s">
+      <c r="F30" s="13" t="s">
         <v>8</v>
       </c>
       <c r="G30" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="H30" s="33" t="s">
+      <c r="H30" s="13" t="s">
         <v>8</v>
       </c>
       <c r="I30" s="3" t="s">
-        <v>67</v>
-      </c>
-    </row>
-    <row r="31" spans="2:19" x14ac:dyDescent="0.3">
-      <c r="B31" s="11">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="31" spans="2:19" x14ac:dyDescent="0.25">
+      <c r="B31" s="6">
         <v>21</v>
       </c>
-      <c r="C31" s="33" t="s">
+      <c r="C31" s="13" t="s">
         <v>32</v>
       </c>
       <c r="D31" s="3" t="s">
@@ -2097,21 +2128,21 @@
       <c r="E31" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="F31" s="33" t="s">
+      <c r="F31" s="13" t="s">
         <v>8</v>
       </c>
       <c r="G31" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="H31" s="33" t="s">
+      <c r="H31" s="13" t="s">
         <v>8</v>
       </c>
       <c r="I31" s="3" t="s">
-        <v>68</v>
-      </c>
-    </row>
-    <row r="32" spans="2:19" x14ac:dyDescent="0.3">
-      <c r="B32" s="11">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="32" spans="2:19" x14ac:dyDescent="0.25">
+      <c r="B32" s="6">
         <v>22</v>
       </c>
       <c r="C32" s="3" t="s">
@@ -2133,11 +2164,11 @@
         <v>9</v>
       </c>
       <c r="I32" s="3" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="33" spans="2:9" x14ac:dyDescent="0.3">
-      <c r="B33" s="11">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="33" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B33" s="6">
         <v>23</v>
       </c>
       <c r="C33" s="3" t="s">
@@ -2159,15 +2190,15 @@
         <v>9</v>
       </c>
       <c r="I33" s="3" t="s">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="34" spans="2:9" x14ac:dyDescent="0.3">
-      <c r="B34" s="11">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="34" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B34" s="6">
         <v>24</v>
       </c>
       <c r="C34" s="3" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="D34" s="3" t="s">
         <v>12</v>
@@ -2185,15 +2216,15 @@
         <v>9</v>
       </c>
       <c r="I34" s="3" t="s">
-        <v>93</v>
-      </c>
-    </row>
-    <row r="35" spans="2:9" x14ac:dyDescent="0.3">
-      <c r="B35" s="11">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="35" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B35" s="6">
         <v>25</v>
       </c>
       <c r="C35" s="3" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="D35" s="3" t="s">
         <v>12</v>
@@ -2211,15 +2242,15 @@
         <v>9</v>
       </c>
       <c r="I35" s="3" t="s">
-        <v>93</v>
-      </c>
-    </row>
-    <row r="36" spans="2:9" x14ac:dyDescent="0.3">
-      <c r="B36" s="11">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="36" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B36" s="6">
         <v>26</v>
       </c>
       <c r="C36" s="3" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
       <c r="D36" s="3" t="s">
         <v>12</v>
@@ -2237,15 +2268,15 @@
         <v>9</v>
       </c>
       <c r="I36" s="3" t="s">
-        <v>93</v>
-      </c>
-    </row>
-    <row r="37" spans="2:9" x14ac:dyDescent="0.3">
-      <c r="B37" s="11">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="37" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B37" s="6">
         <v>27</v>
       </c>
       <c r="C37" s="3" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="D37" s="3" t="s">
         <v>12</v>
@@ -2263,15 +2294,15 @@
         <v>9</v>
       </c>
       <c r="I37" s="3" t="s">
-        <v>93</v>
-      </c>
-    </row>
-    <row r="38" spans="2:9" x14ac:dyDescent="0.3">
-      <c r="B38" s="11">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="38" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B38" s="6">
         <v>28</v>
       </c>
       <c r="C38" s="3" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="D38" s="3" t="s">
         <v>12</v>
@@ -2289,89 +2320,89 @@
         <v>9</v>
       </c>
       <c r="I38" s="3" t="s">
-        <v>93</v>
-      </c>
-    </row>
-    <row r="39" spans="2:9" x14ac:dyDescent="0.3">
-      <c r="B39" s="11">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="39" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B39" s="6">
         <v>29</v>
       </c>
       <c r="C39" s="3" t="s">
+        <v>87</v>
+      </c>
+      <c r="D39" s="3" t="s">
+        <v>102</v>
+      </c>
+      <c r="E39" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="F39" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="G39" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="H39" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="I39" s="3" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="40" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B40" s="6">
+        <v>30</v>
+      </c>
+      <c r="C40" s="3" t="s">
+        <v>88</v>
+      </c>
+      <c r="D40" s="3" t="s">
+        <v>102</v>
+      </c>
+      <c r="E40" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="F40" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="G40" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="H40" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="I40" s="3" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="41" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B41" s="6">
+        <v>31</v>
+      </c>
+      <c r="C41" s="3" t="s">
         <v>89</v>
       </c>
-      <c r="D39" s="3" t="s">
-        <v>104</v>
-      </c>
-      <c r="E39" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="F39" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="G39" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="H39" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="I39" s="3" t="s">
-        <v>92</v>
-      </c>
-    </row>
-    <row r="40" spans="2:9" x14ac:dyDescent="0.3">
-      <c r="B40" s="11">
-        <v>30</v>
-      </c>
-      <c r="C40" s="3" t="s">
+      <c r="D41" s="3" t="s">
+        <v>102</v>
+      </c>
+      <c r="E41" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="F41" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="G41" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="H41" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="I41" s="3" t="s">
         <v>90</v>
       </c>
-      <c r="D40" s="3" t="s">
-        <v>104</v>
-      </c>
-      <c r="E40" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="F40" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="G40" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="H40" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="I40" s="3" t="s">
-        <v>92</v>
-      </c>
-    </row>
-    <row r="41" spans="2:9" x14ac:dyDescent="0.3">
-      <c r="B41" s="11">
-        <v>31</v>
-      </c>
-      <c r="C41" s="3" t="s">
-        <v>91</v>
-      </c>
-      <c r="D41" s="3" t="s">
-        <v>104</v>
-      </c>
-      <c r="E41" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="F41" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="G41" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="H41" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="I41" s="3" t="s">
-        <v>92</v>
-      </c>
-    </row>
-    <row r="42" spans="2:9" x14ac:dyDescent="0.3">
-      <c r="B42" s="11">
+    </row>
+    <row r="42" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B42" s="6">
         <v>32</v>
       </c>
       <c r="C42" s="3" t="s">
@@ -2393,11 +2424,11 @@
         <v>9</v>
       </c>
       <c r="I42" s="3" t="s">
-        <v>71</v>
-      </c>
-    </row>
-    <row r="43" spans="2:9" x14ac:dyDescent="0.3">
-      <c r="B43" s="11">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="43" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B43" s="6">
         <v>33</v>
       </c>
       <c r="C43" s="3" t="s">
@@ -2419,11 +2450,11 @@
         <v>9</v>
       </c>
       <c r="I43" s="3" t="s">
-        <v>72</v>
-      </c>
-    </row>
-    <row r="44" spans="2:9" x14ac:dyDescent="0.3">
-      <c r="B44" s="11">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="44" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B44" s="6">
         <v>34</v>
       </c>
       <c r="C44" s="3" t="s">
@@ -2445,11 +2476,11 @@
         <v>9</v>
       </c>
       <c r="I44" s="3" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="B10:I44" xr:uid="{7E62206A-A624-4BB5-A9AA-3D9B15133065}"/>
+  <autoFilter ref="B10:I44"/>
   <mergeCells count="8">
     <mergeCell ref="L8:S8"/>
     <mergeCell ref="L9:S9"/>
@@ -2466,176 +2497,176 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E8CD7269-9C27-4517-9AB0-2FCC83015950}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B3:G15"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="3.6640625" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="3.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="3.44140625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="14.5546875" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="14.77734375" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="15.44140625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="11.77734375" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="9.5546875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="3.42578125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="14.5703125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="14.7109375" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="15.42578125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="11.7109375" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="9.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="3" spans="2:7" x14ac:dyDescent="0.3">
-      <c r="B3" s="17" t="s">
+    <row r="3" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B3" s="9" t="s">
         <v>2</v>
       </c>
-      <c r="C3" s="13" t="s">
+      <c r="C3" s="8" t="s">
+        <v>73</v>
+      </c>
+      <c r="D3" s="8" t="s">
+        <v>74</v>
+      </c>
+      <c r="E3" s="8" t="s">
         <v>75</v>
       </c>
-      <c r="D3" s="13" t="s">
+      <c r="F3" s="8" t="s">
+        <v>99</v>
+      </c>
+      <c r="G3" s="8" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="4" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B4" s="10">
+        <v>1</v>
+      </c>
+      <c r="C4" s="8" t="s">
         <v>76</v>
       </c>
-      <c r="E3" s="13" t="s">
+      <c r="D4" s="8" t="s">
         <v>77</v>
       </c>
-      <c r="F3" s="13" t="s">
-        <v>101</v>
-      </c>
-      <c r="G3" s="13" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="4" spans="2:7" x14ac:dyDescent="0.3">
-      <c r="B4" s="18">
-        <v>1</v>
-      </c>
-      <c r="C4" s="13" t="s">
+      <c r="E4" s="8" t="s">
         <v>78</v>
       </c>
-      <c r="D4" s="13" t="s">
+      <c r="F4" s="8" t="s">
+        <v>8</v>
+      </c>
+      <c r="G4" s="8"/>
+    </row>
+    <row r="5" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B5" s="11">
+        <v>2</v>
+      </c>
+      <c r="C5" s="8" t="s">
+        <v>76</v>
+      </c>
+      <c r="D5" s="8" t="s">
+        <v>77</v>
+      </c>
+      <c r="E5" s="8" t="s">
         <v>79</v>
       </c>
-      <c r="E4" s="13" t="s">
-        <v>80</v>
-      </c>
-      <c r="F4" s="13" t="s">
+      <c r="F5" s="8" t="s">
         <v>8</v>
       </c>
-      <c r="G4" s="13"/>
-    </row>
-    <row r="5" spans="2:7" x14ac:dyDescent="0.3">
-      <c r="B5" s="19">
-        <v>2</v>
-      </c>
-      <c r="C5" s="13" t="s">
-        <v>78</v>
-      </c>
-      <c r="D5" s="13" t="s">
-        <v>79</v>
-      </c>
-      <c r="E5" s="13" t="s">
-        <v>81</v>
-      </c>
-      <c r="F5" s="13" t="s">
+      <c r="G5" s="8"/>
+    </row>
+    <row r="6" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B6" s="10">
+        <v>3</v>
+      </c>
+      <c r="C6" s="8"/>
+      <c r="D6" s="8"/>
+      <c r="E6" s="8"/>
+      <c r="F6" s="8"/>
+      <c r="G6" s="8"/>
+    </row>
+    <row r="7" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B7" s="11">
+        <v>4</v>
+      </c>
+      <c r="C7" s="8"/>
+      <c r="D7" s="8"/>
+      <c r="E7" s="8"/>
+      <c r="F7" s="8"/>
+      <c r="G7" s="8"/>
+    </row>
+    <row r="8" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B8" s="10">
+        <v>5</v>
+      </c>
+      <c r="C8" s="8"/>
+      <c r="D8" s="8"/>
+      <c r="E8" s="8"/>
+      <c r="F8" s="8"/>
+      <c r="G8" s="8"/>
+    </row>
+    <row r="9" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B9" s="11">
+        <v>6</v>
+      </c>
+      <c r="C9" s="8"/>
+      <c r="D9" s="8"/>
+      <c r="E9" s="8"/>
+      <c r="F9" s="8"/>
+      <c r="G9" s="8"/>
+    </row>
+    <row r="10" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B10" s="10">
+        <v>7</v>
+      </c>
+      <c r="C10" s="8"/>
+      <c r="D10" s="8"/>
+      <c r="E10" s="8"/>
+      <c r="F10" s="8"/>
+      <c r="G10" s="8"/>
+    </row>
+    <row r="11" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B11" s="11">
         <v>8</v>
       </c>
-      <c r="G5" s="13"/>
-    </row>
-    <row r="6" spans="2:7" x14ac:dyDescent="0.3">
-      <c r="B6" s="18">
-        <v>3</v>
-      </c>
-      <c r="C6" s="13"/>
-      <c r="D6" s="13"/>
-      <c r="E6" s="13"/>
-      <c r="F6" s="13"/>
-      <c r="G6" s="13"/>
-    </row>
-    <row r="7" spans="2:7" x14ac:dyDescent="0.3">
-      <c r="B7" s="19">
-        <v>4</v>
-      </c>
-      <c r="C7" s="13"/>
-      <c r="D7" s="13"/>
-      <c r="E7" s="13"/>
-      <c r="F7" s="13"/>
-      <c r="G7" s="13"/>
-    </row>
-    <row r="8" spans="2:7" x14ac:dyDescent="0.3">
-      <c r="B8" s="18">
-        <v>5</v>
-      </c>
-      <c r="C8" s="13"/>
-      <c r="D8" s="13"/>
-      <c r="E8" s="13"/>
-      <c r="F8" s="13"/>
-      <c r="G8" s="13"/>
-    </row>
-    <row r="9" spans="2:7" x14ac:dyDescent="0.3">
-      <c r="B9" s="19">
-        <v>6</v>
-      </c>
-      <c r="C9" s="13"/>
-      <c r="D9" s="13"/>
-      <c r="E9" s="13"/>
-      <c r="F9" s="13"/>
-      <c r="G9" s="13"/>
-    </row>
-    <row r="10" spans="2:7" x14ac:dyDescent="0.3">
-      <c r="B10" s="18">
-        <v>7</v>
-      </c>
-      <c r="C10" s="13"/>
-      <c r="D10" s="13"/>
-      <c r="E10" s="13"/>
-      <c r="F10" s="13"/>
-      <c r="G10" s="13"/>
-    </row>
-    <row r="11" spans="2:7" x14ac:dyDescent="0.3">
-      <c r="B11" s="19">
-        <v>8</v>
-      </c>
-      <c r="C11" s="13"/>
-      <c r="D11" s="13"/>
-      <c r="E11" s="13"/>
-      <c r="F11" s="13"/>
-      <c r="G11" s="13"/>
-    </row>
-    <row r="12" spans="2:7" x14ac:dyDescent="0.3">
-      <c r="B12" s="18">
-        <v>9</v>
-      </c>
-      <c r="C12" s="13"/>
-      <c r="D12" s="13"/>
-      <c r="E12" s="13"/>
-      <c r="F12" s="13"/>
-      <c r="G12" s="13"/>
-    </row>
-    <row r="13" spans="2:7" x14ac:dyDescent="0.3">
-      <c r="B13" s="19">
+      <c r="C11" s="8"/>
+      <c r="D11" s="8"/>
+      <c r="E11" s="8"/>
+      <c r="F11" s="8"/>
+      <c r="G11" s="8"/>
+    </row>
+    <row r="12" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B12" s="10">
+        <v>9</v>
+      </c>
+      <c r="C12" s="8"/>
+      <c r="D12" s="8"/>
+      <c r="E12" s="8"/>
+      <c r="F12" s="8"/>
+      <c r="G12" s="8"/>
+    </row>
+    <row r="13" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B13" s="11">
         <v>10</v>
       </c>
-      <c r="C13" s="13"/>
-      <c r="D13" s="13"/>
-      <c r="E13" s="13"/>
-      <c r="F13" s="13"/>
-      <c r="G13" s="13"/>
-    </row>
-    <row r="14" spans="2:7" x14ac:dyDescent="0.3">
-      <c r="B14" s="18">
+      <c r="C13" s="8"/>
+      <c r="D13" s="8"/>
+      <c r="E13" s="8"/>
+      <c r="F13" s="8"/>
+      <c r="G13" s="8"/>
+    </row>
+    <row r="14" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B14" s="10">
         <v>11</v>
       </c>
-      <c r="C14" s="13"/>
-      <c r="D14" s="13"/>
-      <c r="E14" s="13"/>
-      <c r="F14" s="13"/>
-      <c r="G14" s="13"/>
-    </row>
-    <row r="15" spans="2:7" x14ac:dyDescent="0.3">
-      <c r="B15" s="19">
+      <c r="C14" s="8"/>
+      <c r="D14" s="8"/>
+      <c r="E14" s="8"/>
+      <c r="F14" s="8"/>
+      <c r="G14" s="8"/>
+    </row>
+    <row r="15" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B15" s="11">
         <v>12</v>
       </c>
-      <c r="C15" s="13"/>
-      <c r="D15" s="13"/>
-      <c r="E15" s="13"/>
-      <c r="F15" s="13"/>
-      <c r="G15" s="13"/>
+      <c r="C15" s="8"/>
+      <c r="D15" s="8"/>
+      <c r="E15" s="8"/>
+      <c r="F15" s="8"/>
+      <c r="G15" s="8"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -2643,4 +2674,313 @@
     <tablePart r:id="rId1"/>
   </tableParts>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:F15"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E13" sqref="E13"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="12.42578125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="20.7109375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="41.7109375" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A2" s="6" t="s">
+        <v>81</v>
+      </c>
+      <c r="B2" s="3" t="s">
+        <v>113</v>
+      </c>
+      <c r="C2" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A3" s="13" t="s">
+        <v>82</v>
+      </c>
+      <c r="B3" s="3" t="s">
+        <v>107</v>
+      </c>
+      <c r="C3" t="s">
+        <v>106</v>
+      </c>
+      <c r="D3" t="s">
+        <v>114</v>
+      </c>
+      <c r="E3" t="s">
+        <v>115</v>
+      </c>
+      <c r="F3" t="str">
+        <f>CONCATENATE(C3,E3,A3,E3,B3,D3)</f>
+        <v>ALTER TABLE public.mst_global ADD COLUMN type character varying(15);</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A4" s="3" t="s">
+        <v>83</v>
+      </c>
+      <c r="B4" s="3" t="s">
+        <v>108</v>
+      </c>
+      <c r="C4" t="s">
+        <v>106</v>
+      </c>
+      <c r="D4" t="s">
+        <v>114</v>
+      </c>
+      <c r="E4" t="s">
+        <v>115</v>
+      </c>
+      <c r="F4" t="str">
+        <f t="shared" ref="F4:F15" si="0">CONCATENATE(C4,E4,A4,E4,B4,D4)</f>
+        <v>ALTER TABLE public.mst_global ADD COLUMN description character varying(300);</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A5" s="3" t="s">
+        <v>84</v>
+      </c>
+      <c r="B5" s="3" t="s">
+        <v>109</v>
+      </c>
+      <c r="C5" t="s">
+        <v>106</v>
+      </c>
+      <c r="D5" t="s">
+        <v>114</v>
+      </c>
+      <c r="E5" t="s">
+        <v>115</v>
+      </c>
+      <c r="F5" t="str">
+        <f t="shared" si="0"/>
+        <v>ALTER TABLE public.mst_global ADD COLUMN segment1 character varying(100);</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A6" s="3" t="s">
+        <v>85</v>
+      </c>
+      <c r="B6" s="3" t="s">
+        <v>109</v>
+      </c>
+      <c r="C6" t="s">
+        <v>106</v>
+      </c>
+      <c r="D6" t="s">
+        <v>114</v>
+      </c>
+      <c r="E6" t="s">
+        <v>115</v>
+      </c>
+      <c r="F6" t="str">
+        <f t="shared" si="0"/>
+        <v>ALTER TABLE public.mst_global ADD COLUMN segment2 character varying(100);</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A7" s="3" t="s">
+        <v>86</v>
+      </c>
+      <c r="B7" s="3" t="s">
+        <v>109</v>
+      </c>
+      <c r="C7" t="s">
+        <v>106</v>
+      </c>
+      <c r="D7" t="s">
+        <v>114</v>
+      </c>
+      <c r="E7" t="s">
+        <v>115</v>
+      </c>
+      <c r="F7" t="str">
+        <f t="shared" si="0"/>
+        <v>ALTER TABLE public.mst_global ADD COLUMN segment3 character varying(100);</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A8" s="3" t="s">
+        <v>87</v>
+      </c>
+      <c r="B8" s="3" t="s">
+        <v>111</v>
+      </c>
+      <c r="C8" t="s">
+        <v>106</v>
+      </c>
+      <c r="D8" t="s">
+        <v>114</v>
+      </c>
+      <c r="E8" t="s">
+        <v>115</v>
+      </c>
+      <c r="F8" t="str">
+        <f t="shared" si="0"/>
+        <v>ALTER TABLE public.mst_global ADD COLUMN num1 interger;</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A9" s="3" t="s">
+        <v>88</v>
+      </c>
+      <c r="B9" s="3" t="s">
+        <v>111</v>
+      </c>
+      <c r="C9" t="s">
+        <v>106</v>
+      </c>
+      <c r="D9" t="s">
+        <v>114</v>
+      </c>
+      <c r="E9" t="s">
+        <v>115</v>
+      </c>
+      <c r="F9" t="str">
+        <f t="shared" si="0"/>
+        <v>ALTER TABLE public.mst_global ADD COLUMN num2 interger;</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A10" s="3" t="s">
+        <v>89</v>
+      </c>
+      <c r="B10" s="3" t="s">
+        <v>111</v>
+      </c>
+      <c r="C10" t="s">
+        <v>106</v>
+      </c>
+      <c r="D10" t="s">
+        <v>114</v>
+      </c>
+      <c r="E10" t="s">
+        <v>115</v>
+      </c>
+      <c r="F10" t="str">
+        <f t="shared" si="0"/>
+        <v>ALTER TABLE public.mst_global ADD COLUMN num3 interger;</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A11" s="3" t="s">
+        <v>97</v>
+      </c>
+      <c r="B11" s="3" t="s">
+        <v>108</v>
+      </c>
+      <c r="C11" t="s">
+        <v>106</v>
+      </c>
+      <c r="D11" t="s">
+        <v>114</v>
+      </c>
+      <c r="E11" t="s">
+        <v>115</v>
+      </c>
+      <c r="F11" t="str">
+        <f t="shared" si="0"/>
+        <v>ALTER TABLE public.mst_global ADD COLUMN note character varying(300);</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A12" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="B12" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="C12" t="s">
+        <v>106</v>
+      </c>
+      <c r="D12" t="s">
+        <v>114</v>
+      </c>
+      <c r="E12" t="s">
+        <v>115</v>
+      </c>
+      <c r="F12" t="str">
+        <f t="shared" si="0"/>
+        <v>ALTER TABLE public.mst_global ADD COLUMN flag_active boolean;</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A13" s="3" t="s">
+        <v>94</v>
+      </c>
+      <c r="B13" s="3" t="s">
+        <v>110</v>
+      </c>
+      <c r="C13" t="s">
+        <v>106</v>
+      </c>
+      <c r="D13" t="s">
+        <v>114</v>
+      </c>
+      <c r="E13" t="s">
+        <v>115</v>
+      </c>
+      <c r="F13" t="str">
+        <f t="shared" si="0"/>
+        <v>ALTER TABLE public.mst_global ADD COLUMN user_update character varying(20);</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A14" s="3" t="s">
+        <v>95</v>
+      </c>
+      <c r="B14" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="C14" t="s">
+        <v>106</v>
+      </c>
+      <c r="D14" t="s">
+        <v>114</v>
+      </c>
+      <c r="E14" t="s">
+        <v>115</v>
+      </c>
+      <c r="F14" t="str">
+        <f t="shared" si="0"/>
+        <v>ALTER TABLE public.mst_global ADD COLUMN date_update date;</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A15" s="3" t="s">
+        <v>96</v>
+      </c>
+      <c r="B15" s="3" t="s">
+        <v>112</v>
+      </c>
+      <c r="C15" t="s">
+        <v>106</v>
+      </c>
+      <c r="D15" t="s">
+        <v>114</v>
+      </c>
+      <c r="E15" t="s">
+        <v>115</v>
+      </c>
+      <c r="F15" t="str">
+        <f t="shared" si="0"/>
+        <v>ALTER TABLE public.mst_global ADD COLUMN time_update timestamp without zone;</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>